<commit_message>
evaluasi hasil audit SPI
</commit_message>
<xml_diff>
--- a/Nitip file/Notasi Audit LNO/Evaluasi hasil edit SPI.xlsx
+++ b/Nitip file/Notasi Audit LNO/Evaluasi hasil edit SPI.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9931" uniqueCount="2299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9932" uniqueCount="2300">
   <si>
     <t>900. Kantor Pusat</t>
   </si>
@@ -6923,6 +6923,9 @@
   </si>
   <si>
     <t>Bayu Wibowo Putera</t>
+  </si>
+  <si>
+    <t>disamakan dgn bpk Latif</t>
   </si>
 </sst>
 </file>
@@ -6938,12 +6941,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -6973,7 +6994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6986,6 +7007,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -63947,10 +63971,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63960,9 +63984,10 @@
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>2145</v>
       </c>
@@ -63973,11 +63998,11 @@
         <v>2147</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2136</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>2134</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -63989,8 +64014,11 @@
       <c r="E2" t="s">
         <v>2282</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>2299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" t="s">
         <v>139</v>
@@ -64005,7 +64033,7 @@
         <v>2281</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>1335</v>
@@ -64020,9 +64048,9 @@
         <v>2281</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>2135</v>
       </c>
       <c r="C5" t="s">
@@ -64035,7 +64063,7 @@
         <v>2282</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2137</v>
       </c>
@@ -64052,7 +64080,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2139</v>
       </c>
@@ -64066,7 +64094,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2140</v>
       </c>
@@ -64080,7 +64108,7 @@
         <v>2282</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>1578</v>
       </c>
@@ -64091,10 +64119,10 @@
         <v>2282</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2282</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>2141</v>
       </c>
@@ -64108,7 +64136,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>1413</v>
       </c>
@@ -64122,7 +64150,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>864</v>
       </c>
@@ -64136,7 +64164,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>1344</v>
       </c>
@@ -64150,7 +64178,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2142</v>
       </c>
@@ -64164,7 +64192,7 @@
         <v>2282</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>2143</v>
       </c>
@@ -64178,7 +64206,7 @@
         <v>2282</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>2077</v>
       </c>
@@ -64193,7 +64221,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
         <v>2144</v>
       </c>
       <c r="C17" t="s">
@@ -64266,7 +64294,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="B22" s="8" t="s">
         <v>1481</v>
       </c>
       <c r="C22" t="s">
@@ -64294,7 +64322,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="B24" s="8" t="s">
         <v>2197</v>
       </c>
       <c r="C24" t="s">
@@ -64350,7 +64378,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="B28" s="8" t="s">
         <v>2288</v>
       </c>
       <c r="C28" t="s">
@@ -64462,7 +64490,7 @@
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="B36" s="8" t="s">
         <v>1810</v>
       </c>
       <c r="C36" t="s">
@@ -64504,7 +64532,7 @@
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="B39" s="8" t="s">
         <v>2297</v>
       </c>
       <c r="C39" t="s">
@@ -64532,7 +64560,7 @@
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+      <c r="B41" s="8" t="s">
         <v>1727</v>
       </c>
       <c r="C41" t="s">

</xml_diff>